<commit_message>
file changes for test
</commit_message>
<xml_diff>
--- a/My_Data/My_TEST_Copy.xlsx
+++ b/My_Data/My_TEST_Copy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="About_Me_Dtls1" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -100,7 +100,7 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FFC9211E"/>
+      <color rgb="FF1C1C1C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -109,6 +109,14 @@
       <i val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -156,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,6 +203,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -263,7 +275,7 @@
       <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF1C1C1C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -276,8 +288,8 @@
   </sheetPr>
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,18 +397,7 @@
         <v>MALE</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>555</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <f aca="false">A8-B8</f>
-        <v>-550</v>
-      </c>
-    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G17" s="1" t="s">
         <v>8</v>
@@ -420,8 +421,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -441,7 +442,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>

</xml_diff>